<commit_message>
Create Leisure Facilities Universe spreadsheet
</commit_message>
<xml_diff>
--- a/£BOWL.xlsx
+++ b/£BOWL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8562CE30-82F3-4FF9-B370-BA1E3C7F2433}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037B2EDE-96D1-4D98-9829-F48393B98C23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{4835F308-E20A-4B7A-9F17-94D4123EA96B}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="149">
   <si>
     <t>£BOWL</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Hemel, UK</t>
   </si>
   <si>
-    <t>2015?</t>
-  </si>
-  <si>
     <t>IR</t>
   </si>
   <si>
@@ -408,9 +405,6 @@
     <t>Laurence Keen</t>
   </si>
   <si>
-    <t>Metrics</t>
-  </si>
-  <si>
     <t>Hollywood Bowl</t>
   </si>
   <si>
@@ -550,6 +544,21 @@
   </si>
   <si>
     <t>ROCE</t>
+  </si>
+  <si>
+    <t>Non-Finance Metrics</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Directors</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>Operations</t>
   </si>
 </sst>
 </file>
@@ -889,7 +898,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1125,6 +1134,12 @@
     <xf numFmtId="165" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="15" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="168" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1134,28 +1149,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1174,6 +1171,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1273,7 +1299,7 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1323,7 +1349,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1377,7 +1403,7 @@
       <sheetData sheetId="0">
         <row r="25">
           <cell r="C25">
-            <v>47</v>
+            <v>48</v>
           </cell>
         </row>
       </sheetData>
@@ -1691,7 +1717,7 @@
   <dimension ref="B2:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C27" sqref="C27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1711,27 +1737,27 @@
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
-      <c r="H5" s="143" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
-      <c r="K5" s="144"/>
-      <c r="L5" s="145"/>
-      <c r="O5" s="143" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" s="144"/>
-      <c r="Q5" s="144"/>
-      <c r="R5" s="144"/>
-      <c r="S5" s="144"/>
-      <c r="T5" s="144"/>
-      <c r="U5" s="145"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="147"/>
+      <c r="H5" s="145" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="146"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="146"/>
+      <c r="L5" s="147"/>
+      <c r="O5" s="145" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="146"/>
+      <c r="Q5" s="146"/>
+      <c r="R5" s="146"/>
+      <c r="S5" s="146"/>
+      <c r="T5" s="146"/>
+      <c r="U5" s="147"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
@@ -1741,20 +1767,20 @@
         <v>2.3650000000000002</v>
       </c>
       <c r="D6" s="39"/>
-      <c r="H6" s="154" t="s">
-        <v>105</v>
-      </c>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
-      <c r="K6" s="155"/>
+      <c r="H6" s="150" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="151"/>
+      <c r="J6" s="151"/>
+      <c r="K6" s="151"/>
       <c r="L6" s="58" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O6" s="92">
         <v>44866</v>
       </c>
       <c r="P6" s="93" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
@@ -1774,15 +1800,15 @@
         <f>$C$28</f>
         <v>FY22</v>
       </c>
-      <c r="H7" s="156" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" s="157"/>
-      <c r="J7" s="157"/>
-      <c r="K7" s="157"/>
+      <c r="H7" s="152" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
       <c r="L7" s="59">
         <f>[1]Main!$C$25</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O7" s="17"/>
       <c r="P7" s="6"/>
@@ -1801,12 +1827,12 @@
         <v>404.29506139000006</v>
       </c>
       <c r="D8" s="39"/>
-      <c r="H8" s="158" t="s">
-        <v>106</v>
-      </c>
-      <c r="I8" s="152"/>
-      <c r="J8" s="152"/>
-      <c r="K8" s="152"/>
+      <c r="H8" s="154" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="143"/>
+      <c r="J8" s="143"/>
+      <c r="K8" s="143"/>
       <c r="L8" s="59">
         <v>11</v>
       </c>
@@ -1823,19 +1849,19 @@
         <v>6</v>
       </c>
       <c r="C9" s="14">
-        <f>'Financial Model'!V63</f>
+        <f>'Financial Model'!V67</f>
         <v>56.066000000000003</v>
       </c>
       <c r="D9" s="39" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$28</f>
         <v>FY22</v>
       </c>
-      <c r="H9" s="158" t="s">
-        <v>107</v>
-      </c>
-      <c r="I9" s="152"/>
-      <c r="J9" s="152"/>
-      <c r="K9" s="152"/>
+      <c r="H9" s="154" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="143"/>
+      <c r="J9" s="143"/>
+      <c r="K9" s="143"/>
       <c r="L9" s="59">
         <v>6</v>
       </c>
@@ -1852,19 +1878,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="14">
-        <f>'Financial Model'!V64</f>
+        <f>'Financial Model'!V68</f>
         <v>0</v>
       </c>
       <c r="D10" s="39" t="str">
         <f t="shared" si="0"/>
         <v>FY22</v>
       </c>
-      <c r="H10" s="158" t="s">
-        <v>108</v>
-      </c>
-      <c r="I10" s="152"/>
-      <c r="J10" s="152"/>
-      <c r="K10" s="152"/>
+      <c r="H10" s="154" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" s="143"/>
+      <c r="J10" s="143"/>
+      <c r="K10" s="143"/>
       <c r="L10" s="59">
         <v>7</v>
       </c>
@@ -1888,12 +1914,12 @@
         <f t="shared" si="0"/>
         <v>FY22</v>
       </c>
-      <c r="H11" s="158" t="s">
-        <v>109</v>
-      </c>
-      <c r="I11" s="152"/>
-      <c r="J11" s="152"/>
-      <c r="K11" s="152"/>
+      <c r="H11" s="154" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="143"/>
+      <c r="J11" s="143"/>
+      <c r="K11" s="143"/>
       <c r="L11" s="59">
         <v>6</v>
       </c>
@@ -1914,12 +1940,12 @@
         <v>348.22906139000008</v>
       </c>
       <c r="D12" s="40"/>
-      <c r="H12" s="159" t="s">
-        <v>110</v>
-      </c>
-      <c r="I12" s="150"/>
-      <c r="J12" s="150"/>
-      <c r="K12" s="150"/>
+      <c r="H12" s="155" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="148"/>
+      <c r="J12" s="148"/>
+      <c r="K12" s="148"/>
       <c r="L12" s="60">
         <v>174</v>
       </c>
@@ -1953,43 +1979,43 @@
       <c r="U14" s="9"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="143" t="s">
+      <c r="B15" s="145" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="144"/>
-      <c r="D15" s="145"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="147"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="152" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="153"/>
+      <c r="C16" s="143" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="144"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="143" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="152" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="153"/>
-      <c r="H17" s="143" t="s">
-        <v>127</v>
-      </c>
-      <c r="I17" s="144"/>
-      <c r="J17" s="144"/>
-      <c r="K17" s="144"/>
-      <c r="L17" s="145"/>
+      <c r="D17" s="144"/>
+      <c r="H17" s="145" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="146"/>
+      <c r="J17" s="146"/>
+      <c r="K17" s="146"/>
+      <c r="L17" s="147"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18" s="16"/>
-      <c r="C18" s="152"/>
-      <c r="D18" s="153"/>
+      <c r="C18" s="143"/>
+      <c r="D18" s="144"/>
       <c r="H18" s="82" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I18" s="83"/>
       <c r="J18" s="83"/>
@@ -1998,10 +2024,10 @@
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B19" s="50"/>
-      <c r="C19" s="150"/>
-      <c r="D19" s="151"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="149"/>
       <c r="H19" s="86" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I19" s="83"/>
       <c r="J19" s="83"/>
@@ -2015,29 +2041,29 @@
       <c r="K20" s="6"/>
       <c r="L20" s="7"/>
       <c r="P20" s="89" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="H21" s="82" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I21" s="83"/>
       <c r="J21" s="83"/>
       <c r="K21" s="6"/>
       <c r="L21" s="7"/>
       <c r="P21" s="89" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="143" t="s">
+      <c r="B22" s="145" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="144"/>
-      <c r="D22" s="145"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="147"/>
       <c r="H22" s="86" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I22" s="83"/>
       <c r="J22" s="83"/>
@@ -2048,12 +2074,12 @@
       <c r="B23" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="152" t="s">
+      <c r="C23" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="153"/>
+      <c r="D23" s="144"/>
       <c r="H23" s="87" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I23" s="83"/>
       <c r="J23" s="83"/>
@@ -2064,10 +2090,10 @@
       <c r="B24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="152" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="153"/>
+      <c r="C24" s="143">
+        <v>2010</v>
+      </c>
+      <c r="D24" s="144"/>
       <c r="H24" s="82"/>
       <c r="I24" s="83"/>
       <c r="J24" s="83"/>
@@ -2076,12 +2102,12 @@
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="152">
+        <v>32</v>
+      </c>
+      <c r="C25" s="143">
         <v>64</v>
       </c>
-      <c r="D25" s="153"/>
+      <c r="D25" s="144"/>
       <c r="H25" s="82"/>
       <c r="I25" s="83"/>
       <c r="J25" s="83"/>
@@ -2090,10 +2116,13 @@
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" s="152"/>
-      <c r="D26" s="153"/>
+        <v>114</v>
+      </c>
+      <c r="C26" s="170">
+        <f>'Financial Model'!V33</f>
+        <v>2530</v>
+      </c>
+      <c r="D26" s="144"/>
       <c r="H26" s="84"/>
       <c r="I26" s="85"/>
       <c r="J26" s="85"/>
@@ -2102,16 +2131,16 @@
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="152">
+        <v>118</v>
+      </c>
+      <c r="C27" s="143">
         <v>2016</v>
       </c>
-      <c r="D27" s="153"/>
+      <c r="D27" s="144"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" s="90" t="s">
         <v>23</v>
@@ -2122,23 +2151,23 @@
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="158" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="148" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="149"/>
-      <c r="H29" s="143" t="s">
-        <v>128</v>
-      </c>
-      <c r="I29" s="144"/>
-      <c r="J29" s="144"/>
-      <c r="K29" s="144"/>
-      <c r="L29" s="145"/>
+      <c r="D29" s="159"/>
+      <c r="H29" s="145" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" s="146"/>
+      <c r="J29" s="146"/>
+      <c r="K29" s="146"/>
+      <c r="L29" s="147"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="H30" s="82" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I30" s="83"/>
       <c r="J30" s="83"/>
@@ -2147,7 +2176,7 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="H31" s="86" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I31" s="83"/>
       <c r="J31" s="83"/>
@@ -2155,13 +2184,13 @@
       <c r="L31" s="7"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B32" s="143" t="s">
-        <v>135</v>
-      </c>
-      <c r="C32" s="144"/>
-      <c r="D32" s="145"/>
+      <c r="B32" s="145" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="146"/>
+      <c r="D32" s="147"/>
       <c r="H32" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I32" s="83"/>
       <c r="J32" s="83"/>
@@ -2170,13 +2199,13 @@
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" s="146">
-        <f>C6/'Financial Model'!L61</f>
+        <v>134</v>
+      </c>
+      <c r="C33" s="156">
+        <f>C6/'Financial Model'!L65</f>
         <v>3.0577866054115437</v>
       </c>
-      <c r="D33" s="147"/>
+      <c r="D33" s="157"/>
       <c r="H33" s="86"/>
       <c r="I33" s="83"/>
       <c r="J33" s="83"/>
@@ -2185,15 +2214,15 @@
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B34" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C34" s="146">
+        <v>135</v>
+      </c>
+      <c r="C34" s="156">
         <f>C8/'Financial Model'!U3</f>
         <v>5.6247399954088877</v>
       </c>
-      <c r="D34" s="147"/>
+      <c r="D34" s="157"/>
       <c r="H34" s="82" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I34" s="83"/>
       <c r="J34" s="83"/>
@@ -2202,15 +2231,15 @@
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B35" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="146">
+        <v>136</v>
+      </c>
+      <c r="C35" s="156">
         <f>C6/('Financial Model'!U13*100)</f>
         <v>2.2528786210358729</v>
       </c>
-      <c r="D35" s="147"/>
+      <c r="D35" s="157"/>
       <c r="H35" s="86" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I35" s="83"/>
       <c r="J35" s="83"/>
@@ -2246,14 +2275,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="O5:U5"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="B22:D22"/>
@@ -2268,12 +2295,14 @@
     <mergeCell ref="H11:K11"/>
     <mergeCell ref="H12:K12"/>
     <mergeCell ref="H17:L17"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{A84D86FA-48B5-44CA-921D-0808FAD93C29}"/>
@@ -2288,13 +2317,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EA8208-8B07-4316-8637-70611CF2B90F}">
-  <dimension ref="A1:CR80"/>
+  <dimension ref="A1:CR84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P12" sqref="P12:S12"/>
+      <selection pane="bottomRight" activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2320,16 +2349,16 @@
   <sheetData>
     <row r="1" spans="1:96" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D1" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H1" s="28" t="s">
         <v>14</v>
@@ -2350,10 +2379,10 @@
         <v>19</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R1" s="10" t="s">
         <v>25</v>
@@ -2374,49 +2403,49 @@
         <v>24</v>
       </c>
       <c r="X1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AC1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AD1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AE1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AF1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AI1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AK1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AL1" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="AL1" s="10" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:96" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2469,52 +2498,52 @@
         <v>44834</v>
       </c>
       <c r="W2" s="133" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AD2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AE2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AH2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AI2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AJ2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:96" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2640,7 +2669,7 @@
     <row r="4" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="31"/>
       <c r="F4" s="14">
@@ -2760,7 +2789,7 @@
     <row r="5" spans="1:96" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="12">
@@ -2891,7 +2920,7 @@
     <row r="6" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="14">
@@ -3010,7 +3039,7 @@
     </row>
     <row r="7" spans="1:96" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="14">
@@ -3129,7 +3158,7 @@
     </row>
     <row r="8" spans="1:96" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="12">
@@ -3259,7 +3288,7 @@
     </row>
     <row r="9" spans="1:96" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="14">
@@ -3371,7 +3400,7 @@
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="14">
@@ -3501,7 +3530,7 @@
     </row>
     <row r="11" spans="1:96" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="14">
@@ -3620,7 +3649,7 @@
     </row>
     <row r="12" spans="1:96" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="12">
@@ -3983,7 +4012,7 @@
     </row>
     <row r="13" spans="1:96" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="26">
@@ -4234,7 +4263,7 @@
     </row>
     <row r="15" spans="1:96" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AN15" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AO15" s="62">
         <v>-0.02</v>
@@ -4242,7 +4271,7 @@
     </row>
     <row r="16" spans="1:96" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="34"/>
       <c r="F16" s="23">
@@ -4369,7 +4398,7 @@
         <v>0.86</v>
       </c>
       <c r="AN16" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AO16" s="63">
         <v>7.0000000000000007E-2</v>
@@ -4377,7 +4406,7 @@
     </row>
     <row r="17" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="34"/>
       <c r="F17" s="23">
@@ -4505,7 +4534,7 @@
         <v>0.30209379984489798</v>
       </c>
       <c r="AN17" s="46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AO17" s="64">
         <f>NPV(AO16,X12:CR12)</f>
@@ -4515,7 +4544,7 @@
     <row r="18" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="34"/>
       <c r="F18" s="23">
@@ -4652,7 +4681,7 @@
     </row>
     <row r="19" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E19" s="34"/>
       <c r="F19" s="23">
@@ -4779,7 +4808,7 @@
         <v>0.2</v>
       </c>
       <c r="AN19" s="46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AO19" s="64">
         <f>AO17+AO18</f>
@@ -4788,7 +4817,7 @@
     </row>
     <row r="20" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AN20" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AO20" s="65">
         <f>AO19/Main!C7</f>
@@ -4797,14 +4826,14 @@
     </row>
     <row r="21" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="37"/>
       <c r="F21" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H21" s="23">
         <f t="shared" ref="H21:M21" si="45">H3/F3-1</f>
@@ -4831,7 +4860,7 @@
         <v>0.5227927414761171</v>
       </c>
       <c r="P21" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q21" s="23">
         <f t="shared" ref="Q21:T21" si="46">Q3/P3-1</f>
@@ -4906,7 +4935,7 @@
         <v>0.02</v>
       </c>
       <c r="AN21" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO21" s="67">
         <f>Main!C6</f>
@@ -4916,11 +4945,11 @@
     </row>
     <row r="22" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="34"/>
       <c r="F22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="34">
         <f t="shared" ref="G22" si="48">G3/F3-1</f>
@@ -4951,74 +4980,74 @@
         <v>-6.5935930839647328E-2</v>
       </c>
       <c r="P22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W22" s="138"/>
       <c r="X22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Y22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Z22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AC22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AE22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AF22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AH22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AJ22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AK22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AL22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN22" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AO22" s="66">
         <f>AO20/AO21-1</f>
@@ -5058,7 +5087,7 @@
     </row>
     <row r="24" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="29" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="E24" s="34"/>
       <c r="F24" s="38"/>
@@ -5092,7 +5121,7 @@
     </row>
     <row r="25" spans="1:42" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E25" s="53"/>
       <c r="F25" s="10"/>
@@ -5146,7 +5175,7 @@
     </row>
     <row r="26" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E26" s="34"/>
       <c r="F26" s="38"/>
@@ -5186,7 +5215,7 @@
     </row>
     <row r="27" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S27" s="1">
         <v>6</v>
@@ -5200,7 +5229,7 @@
     </row>
     <row r="28" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
@@ -5239,7 +5268,7 @@
     </row>
     <row r="29" spans="1:42" s="72" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="73" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C29" s="74"/>
       <c r="D29" s="74"/>
@@ -5254,7 +5283,7 @@
       <c r="M29" s="75"/>
       <c r="N29" s="74"/>
       <c r="O29" s="74" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P29" s="81">
         <f>P3/P25</f>
@@ -5289,7 +5318,7 @@
     </row>
     <row r="30" spans="1:42" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="68" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C30" s="69"/>
       <c r="D30" s="69"/>
@@ -5326,7 +5355,7 @@
     </row>
     <row r="31" spans="1:42" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="77" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E31" s="78"/>
       <c r="G31" s="78"/>
@@ -5343,374 +5372,390 @@
       </c>
       <c r="W31" s="79"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B34" s="29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H35" s="14">
-        <v>48.180999999999997</v>
-      </c>
-      <c r="L35" s="14">
-        <v>55.976999999999997</v>
-      </c>
-      <c r="M35" s="31"/>
-      <c r="U35" s="14">
-        <v>49.036000000000001</v>
-      </c>
-      <c r="V35" s="14">
-        <v>68.641000000000005</v>
-      </c>
-      <c r="W35" s="135"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" s="14">
-        <v>147.39099999999999</v>
-      </c>
-      <c r="L36" s="14">
-        <v>133.077</v>
-      </c>
-      <c r="M36" s="31"/>
-      <c r="U36" s="14">
-        <v>132.34200000000001</v>
-      </c>
-      <c r="V36" s="14">
-        <v>147.45500000000001</v>
-      </c>
-      <c r="W36" s="135"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H37" s="14">
-        <v>78.364000000000004</v>
-      </c>
-      <c r="L37" s="14">
-        <v>77.807000000000002</v>
-      </c>
-      <c r="M37" s="31"/>
-      <c r="U37" s="14">
-        <v>77.947999999999993</v>
-      </c>
-      <c r="V37" s="14">
-        <v>81.793999999999997</v>
-      </c>
-      <c r="W37" s="135"/>
+    <row r="32" spans="1:42" s="76" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="77"/>
+      <c r="E32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="I32" s="78"/>
+      <c r="K32" s="78"/>
+      <c r="M32" s="78"/>
+      <c r="P32" s="80"/>
+      <c r="Q32" s="80"/>
+      <c r="W32" s="79"/>
+    </row>
+    <row r="33" spans="1:23" s="160" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="161" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="162"/>
+      <c r="G33" s="162"/>
+      <c r="I33" s="162"/>
+      <c r="K33" s="162"/>
+      <c r="M33" s="162"/>
+      <c r="P33" s="160">
+        <f t="shared" ref="P33:U33" si="51">SUM(P34:P36)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="160">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="R33" s="160">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="S33" s="160">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="T33" s="160">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="U33" s="160">
+        <f t="shared" si="51"/>
+        <v>1787</v>
+      </c>
+      <c r="V33" s="160">
+        <f>SUM(V34:V36)</f>
+        <v>2530</v>
+      </c>
+      <c r="W33" s="163"/>
+    </row>
+    <row r="34" spans="1:23" s="164" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="165" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" s="166"/>
+      <c r="G34" s="166"/>
+      <c r="I34" s="166"/>
+      <c r="K34" s="166"/>
+      <c r="M34" s="166"/>
+      <c r="U34" s="164">
+        <v>6</v>
+      </c>
+      <c r="V34" s="164">
+        <v>7</v>
+      </c>
+      <c r="W34" s="167"/>
+    </row>
+    <row r="35" spans="1:23" s="164" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="165" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="166"/>
+      <c r="G35" s="166"/>
+      <c r="I35" s="166"/>
+      <c r="K35" s="166"/>
+      <c r="M35" s="166"/>
+      <c r="U35" s="164">
+        <v>58</v>
+      </c>
+      <c r="V35" s="164">
+        <v>91</v>
+      </c>
+      <c r="W35" s="167"/>
+    </row>
+    <row r="36" spans="1:23" s="168" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="165" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="169"/>
+      <c r="G36" s="169"/>
+      <c r="I36" s="169"/>
+      <c r="K36" s="169"/>
+      <c r="M36" s="169"/>
+      <c r="U36" s="168">
+        <v>1723</v>
+      </c>
+      <c r="V36" s="168">
+        <v>2432</v>
+      </c>
+      <c r="W36" s="167"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H38" s="14">
-        <v>2.93</v>
-      </c>
-      <c r="L38" s="14">
-        <v>4.13</v>
-      </c>
-      <c r="M38" s="31"/>
-      <c r="U38" s="14">
-        <v>6.29</v>
-      </c>
-      <c r="V38" s="14">
-        <v>1.647</v>
-      </c>
-      <c r="W38" s="135"/>
+      <c r="B38" s="29" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H39" s="14">
-        <f>SUM(H35:H38)</f>
-        <v>276.86600000000004</v>
+        <v>48.180999999999997</v>
       </c>
       <c r="L39" s="14">
-        <f>SUM(L35:L38)</f>
-        <v>270.99099999999999</v>
+        <v>55.976999999999997</v>
       </c>
       <c r="M39" s="31"/>
       <c r="U39" s="14">
-        <f>SUM(U35:U38)</f>
-        <v>265.61600000000004</v>
+        <v>49.036000000000001</v>
       </c>
       <c r="V39" s="14">
-        <f>SUM(V35:V38)</f>
-        <v>299.53699999999998</v>
+        <v>68.641000000000005</v>
       </c>
       <c r="W39" s="135"/>
     </row>
-    <row r="40" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="12">
-        <v>15.635999999999999</v>
-      </c>
-      <c r="I40" s="61"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="12">
-        <v>49.576999999999998</v>
-      </c>
-      <c r="M40" s="30"/>
-      <c r="U40" s="12">
-        <v>29.942</v>
-      </c>
-      <c r="V40" s="12">
-        <v>56.066000000000003</v>
-      </c>
-      <c r="W40" s="134"/>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H40" s="14">
+        <v>147.39099999999999</v>
+      </c>
+      <c r="L40" s="14">
+        <v>133.077</v>
+      </c>
+      <c r="M40" s="31"/>
+      <c r="U40" s="14">
+        <v>132.34200000000001</v>
+      </c>
+      <c r="V40" s="14">
+        <v>147.45500000000001</v>
+      </c>
+      <c r="W40" s="135"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
       <c r="B41" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H41" s="14">
-        <v>2.9940000000000002</v>
+        <v>78.364000000000004</v>
       </c>
       <c r="L41" s="14">
-        <v>10.474</v>
+        <v>77.807000000000002</v>
       </c>
       <c r="M41" s="31"/>
       <c r="U41" s="14">
-        <v>3.3</v>
+        <v>77.947999999999993</v>
       </c>
       <c r="V41" s="14">
-        <v>5.13</v>
+        <v>81.793999999999997</v>
       </c>
       <c r="W41" s="135"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
       <c r="B42" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H42" s="14">
-        <v>1.3120000000000001</v>
+        <v>2.93</v>
       </c>
       <c r="L42" s="14">
-        <v>0</v>
+        <v>4.13</v>
       </c>
       <c r="M42" s="31"/>
       <c r="U42" s="14">
-        <v>0.65</v>
+        <v>6.29</v>
       </c>
       <c r="V42" s="14">
-        <v>0.27100000000000002</v>
+        <v>1.647</v>
       </c>
       <c r="W42" s="135"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
       <c r="B43" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H43" s="14">
-        <v>1.4830000000000001</v>
+        <f>SUM(H39:H42)</f>
+        <v>276.86600000000004</v>
       </c>
       <c r="L43" s="14">
-        <v>1.7390000000000001</v>
+        <f>SUM(L39:L42)</f>
+        <v>270.99099999999999</v>
       </c>
       <c r="M43" s="31"/>
       <c r="U43" s="14">
-        <v>1.4610000000000001</v>
+        <f>SUM(U39:U42)</f>
+        <v>265.61600000000004</v>
       </c>
       <c r="V43" s="14">
-        <v>2.1480000000000001</v>
+        <f>SUM(V39:V42)</f>
+        <v>299.53699999999998</v>
       </c>
       <c r="W43" s="135"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H44" s="14">
-        <f>H39+H40+H41+H42+H43</f>
-        <v>298.29100000000011</v>
-      </c>
-      <c r="L44" s="14">
-        <f>L39+L40+L41+L42+L43</f>
-        <v>332.78099999999995</v>
-      </c>
-      <c r="M44" s="31"/>
-      <c r="U44" s="14">
-        <f>SUM(U40:U43)+U39</f>
-        <v>300.96900000000005</v>
-      </c>
-      <c r="V44" s="14">
-        <f>SUM(V40:V43)+V39</f>
-        <v>363.15199999999999</v>
-      </c>
-      <c r="W44" s="135"/>
+    <row r="44" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="61"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="12">
+        <v>15.635999999999999</v>
+      </c>
+      <c r="I44" s="61"/>
+      <c r="K44" s="61"/>
+      <c r="L44" s="12">
+        <v>49.576999999999998</v>
+      </c>
+      <c r="M44" s="30"/>
+      <c r="U44" s="12">
+        <v>29.942</v>
+      </c>
+      <c r="V44" s="12">
+        <v>56.066000000000003</v>
+      </c>
+      <c r="W44" s="134"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="H45" s="14"/>
-      <c r="L45" s="14"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H45" s="14">
+        <v>2.9940000000000002</v>
+      </c>
+      <c r="L45" s="14">
+        <v>10.474</v>
+      </c>
       <c r="M45" s="31"/>
+      <c r="U45" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="V45" s="14">
+        <v>5.13</v>
+      </c>
+      <c r="W45" s="135"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H46" s="14">
-        <v>11.737</v>
+        <v>1.3120000000000001</v>
       </c>
       <c r="L46" s="14">
-        <v>21.773</v>
+        <v>0</v>
       </c>
       <c r="M46" s="31"/>
       <c r="U46" s="14">
-        <v>18.141999999999999</v>
+        <v>0.65</v>
       </c>
       <c r="V46" s="14">
-        <v>28.681000000000001</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="W46" s="135"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H47" s="14">
-        <v>11.831</v>
+        <v>1.4830000000000001</v>
       </c>
       <c r="L47" s="14">
-        <v>11.615</v>
+        <v>1.7390000000000001</v>
       </c>
       <c r="M47" s="31"/>
       <c r="U47" s="14">
-        <v>13.811</v>
+        <v>1.4610000000000001</v>
       </c>
       <c r="V47" s="14">
-        <v>11.557</v>
+        <v>2.1480000000000001</v>
       </c>
       <c r="W47" s="135"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
       <c r="B48" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H48" s="14">
-        <v>0</v>
+        <f>H43+H44+H45+H46+H47</f>
+        <v>298.29100000000011</v>
       </c>
       <c r="L48" s="14">
-        <v>2.0670000000000002</v>
+        <f>L43+L44+L45+L46+L47</f>
+        <v>332.78099999999995</v>
       </c>
       <c r="M48" s="31"/>
       <c r="U48" s="14">
-        <v>0</v>
+        <f>SUM(U44:U47)+U43</f>
+        <v>300.96900000000005</v>
       </c>
       <c r="V48" s="14">
-        <v>0</v>
+        <f>SUM(V44:V47)+V43</f>
+        <v>363.15199999999999</v>
       </c>
       <c r="W48" s="135"/>
     </row>
-    <row r="49" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="12">
-        <v>5.38</v>
-      </c>
-      <c r="I49" s="61"/>
-      <c r="K49" s="61"/>
-      <c r="L49" s="12">
-        <v>0</v>
-      </c>
-      <c r="M49" s="30"/>
-      <c r="U49" s="12">
-        <v>0</v>
-      </c>
-      <c r="V49" s="12">
-        <v>0</v>
-      </c>
-      <c r="W49" s="134"/>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="H49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="31"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H50" s="14">
-        <f>SUM(H46:H49)</f>
-        <v>28.947999999999997</v>
+        <v>11.737</v>
       </c>
       <c r="L50" s="14">
-        <f>SUM(L46:L49)</f>
-        <v>35.454999999999998</v>
+        <v>21.773</v>
       </c>
       <c r="M50" s="31"/>
       <c r="U50" s="14">
-        <f>SUM(U46:U49)</f>
-        <v>31.952999999999999</v>
+        <v>18.141999999999999</v>
       </c>
       <c r="V50" s="14">
-        <f>SUM(V46:V49)</f>
-        <v>40.238</v>
+        <v>28.681000000000001</v>
       </c>
       <c r="W50" s="135"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
       <c r="B51" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H51" s="14">
-        <v>0.68700000000000006</v>
+        <v>11.831</v>
       </c>
       <c r="L51" s="14">
-        <v>0.51600000000000001</v>
+        <v>11.615</v>
       </c>
       <c r="M51" s="31"/>
       <c r="U51" s="14">
-        <v>0.56499999999999995</v>
+        <v>13.811</v>
       </c>
       <c r="V51" s="14">
-        <v>3</v>
+        <v>11.557</v>
       </c>
       <c r="W51" s="135"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
       <c r="B52" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="H52" s="14">
-        <v>164.32900000000001</v>
+        <v>0</v>
       </c>
       <c r="L52" s="14">
-        <v>160.916</v>
+        <v>2.0670000000000002</v>
       </c>
       <c r="M52" s="31"/>
       <c r="U52" s="14">
-        <v>160.12899999999999</v>
+        <v>0</v>
       </c>
       <c r="V52" s="14">
-        <v>176.81200000000001</v>
+        <v>0</v>
       </c>
       <c r="W52" s="135"/>
     </row>
     <row r="53" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" s="61"/>
       <c r="G53" s="61"/>
       <c r="H53" s="12">
-        <v>24.693000000000001</v>
+        <v>5.38</v>
       </c>
       <c r="I53" s="61"/>
       <c r="K53" s="61"/>
@@ -5729,362 +5774,447 @@
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H54" s="14">
-        <v>3.8029999999999999</v>
+        <f>SUM(H50:H53)</f>
+        <v>28.947999999999997</v>
       </c>
       <c r="L54" s="14">
-        <v>3.7690000000000001</v>
+        <f>SUM(L50:L53)</f>
+        <v>35.454999999999998</v>
       </c>
       <c r="M54" s="31"/>
       <c r="U54" s="14">
-        <v>3.6349999999999998</v>
+        <f>SUM(U50:U53)</f>
+        <v>31.952999999999999</v>
       </c>
       <c r="V54" s="14">
-        <v>4.6820000000000004</v>
+        <f>SUM(V50:V53)</f>
+        <v>40.238</v>
       </c>
       <c r="W54" s="135"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H55" s="14">
-        <f>H50+H51+H52+H53+H54</f>
-        <v>222.46</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="L55" s="14">
-        <f>L50+L51+L52+L53+L54</f>
-        <v>200.65600000000001</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="M55" s="31"/>
       <c r="U55" s="14">
-        <f>U50+U51+U52+U53+U54</f>
-        <v>196.28199999999998</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="V55" s="14">
-        <f>V50+V51+V52+V53+V54</f>
-        <v>224.732</v>
+        <v>3</v>
       </c>
       <c r="W55" s="135"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="H56" s="14"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H57" s="14">
-        <v>75.83</v>
-      </c>
-      <c r="L57" s="14">
-        <v>132.125</v>
-      </c>
-      <c r="M57" s="31"/>
-      <c r="U57" s="14">
-        <v>104.687</v>
-      </c>
-      <c r="V57" s="14">
-        <v>138.41999999999999</v>
-      </c>
-      <c r="W57" s="135"/>
+      <c r="B56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H56" s="14">
+        <v>164.32900000000001</v>
+      </c>
+      <c r="L56" s="14">
+        <v>160.916</v>
+      </c>
+      <c r="M56" s="31"/>
+      <c r="U56" s="14">
+        <v>160.12899999999999</v>
+      </c>
+      <c r="V56" s="14">
+        <v>176.81200000000001</v>
+      </c>
+      <c r="W56" s="135"/>
+    </row>
+    <row r="57" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" s="61"/>
+      <c r="G57" s="61"/>
+      <c r="H57" s="12">
+        <v>24.693000000000001</v>
+      </c>
+      <c r="I57" s="61"/>
+      <c r="K57" s="61"/>
+      <c r="L57" s="12">
+        <v>0</v>
+      </c>
+      <c r="M57" s="30"/>
+      <c r="U57" s="12">
+        <v>0</v>
+      </c>
+      <c r="V57" s="12">
+        <v>0</v>
+      </c>
+      <c r="W57" s="134"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
       <c r="B58" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H58" s="14">
-        <f>H55+H57</f>
-        <v>298.29000000000002</v>
+        <v>3.8029999999999999</v>
       </c>
       <c r="L58" s="14">
-        <f>L55+L57</f>
-        <v>332.78100000000001</v>
+        <v>3.7690000000000001</v>
       </c>
       <c r="M58" s="31"/>
       <c r="U58" s="14">
-        <f>U57+U55</f>
+        <v>3.6349999999999998</v>
+      </c>
+      <c r="V58" s="14">
+        <v>4.6820000000000004</v>
+      </c>
+      <c r="W58" s="135"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59" s="14">
+        <f>H54+H55+H56+H57+H58</f>
+        <v>222.46</v>
+      </c>
+      <c r="L59" s="14">
+        <f>L54+L55+L56+L57+L58</f>
+        <v>200.65600000000001</v>
+      </c>
+      <c r="M59" s="31"/>
+      <c r="U59" s="14">
+        <f>U54+U55+U56+U57+U58</f>
+        <v>196.28199999999998</v>
+      </c>
+      <c r="V59" s="14">
+        <f>V54+V55+V56+V57+V58</f>
+        <v>224.732</v>
+      </c>
+      <c r="W59" s="135"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="H60" s="14"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H61" s="14">
+        <v>75.83</v>
+      </c>
+      <c r="L61" s="14">
+        <v>132.125</v>
+      </c>
+      <c r="M61" s="31"/>
+      <c r="U61" s="14">
+        <v>104.687</v>
+      </c>
+      <c r="V61" s="14">
+        <v>138.41999999999999</v>
+      </c>
+      <c r="W61" s="135"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H62" s="14">
+        <f>H59+H61</f>
+        <v>298.29000000000002</v>
+      </c>
+      <c r="L62" s="14">
+        <f>L59+L61</f>
+        <v>332.78100000000001</v>
+      </c>
+      <c r="M62" s="31"/>
+      <c r="U62" s="14">
+        <f>U61+U59</f>
         <v>300.96899999999999</v>
       </c>
-      <c r="V58" s="14">
-        <f>V57+V55</f>
+      <c r="V62" s="14">
+        <f>V61+V59</f>
         <v>363.15199999999999</v>
       </c>
-      <c r="W58" s="135"/>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H60" s="14">
-        <f>H44-H55</f>
-        <v>75.831000000000103</v>
-      </c>
-      <c r="L60" s="14">
-        <f>L44-L55</f>
-        <v>132.12499999999994</v>
-      </c>
-      <c r="M60" s="31"/>
-      <c r="U60" s="14">
-        <f t="shared" ref="U60:V60" si="51">U44-U55</f>
-        <v>104.68700000000007</v>
-      </c>
-      <c r="V60" s="14">
-        <f t="shared" si="51"/>
-        <v>138.41999999999999</v>
-      </c>
-      <c r="W60" s="135"/>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H61" s="1">
-        <f>H60/H14</f>
-        <v>0.50318915060727853</v>
-      </c>
-      <c r="L61" s="1">
-        <f>L60/L14</f>
-        <v>0.77343526713555533</v>
-      </c>
-      <c r="U61" s="1">
-        <f t="shared" ref="U61:V61" si="52">U60/U14</f>
-        <v>0.63597840274765649</v>
-      </c>
-      <c r="V61" s="1">
-        <f t="shared" si="52"/>
-        <v>0.80971382354881549</v>
-      </c>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B63" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H63" s="14">
-        <f t="shared" ref="H63" si="53">H40</f>
-        <v>15.635999999999999</v>
-      </c>
-      <c r="L63" s="14">
-        <f t="shared" ref="L63" si="54">L40</f>
-        <v>49.576999999999998</v>
-      </c>
-      <c r="U63" s="14">
-        <f t="shared" ref="U63" si="55">U40</f>
-        <v>29.942</v>
-      </c>
-      <c r="V63" s="14">
-        <f>V40</f>
-        <v>56.066000000000003</v>
-      </c>
-      <c r="W63" s="135"/>
+      <c r="W62" s="135"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="H64" s="14">
-        <f t="shared" ref="H64" si="56">H49+H53</f>
-        <v>30.073</v>
+        <f>H48-H59</f>
+        <v>75.831000000000103</v>
       </c>
       <c r="L64" s="14">
-        <f t="shared" ref="L64" si="57">L49+L53</f>
-        <v>0</v>
-      </c>
+        <f>L48-L59</f>
+        <v>132.12499999999994</v>
+      </c>
+      <c r="M64" s="31"/>
       <c r="U64" s="14">
-        <f t="shared" ref="U64" si="58">U49+U53</f>
-        <v>0</v>
+        <f t="shared" ref="U64:V64" si="52">U48-U59</f>
+        <v>104.68700000000007</v>
       </c>
       <c r="V64" s="14">
-        <f>V49+V53</f>
-        <v>0</v>
+        <f t="shared" si="52"/>
+        <v>138.41999999999999</v>
       </c>
       <c r="W64" s="135"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
       <c r="B65" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H65" s="14">
-        <f>H63-H64</f>
-        <v>-14.437000000000001</v>
-      </c>
-      <c r="L65" s="14">
-        <f>L63-L64</f>
-        <v>49.576999999999998</v>
-      </c>
-      <c r="U65" s="14">
-        <f>U63-U64</f>
-        <v>29.942</v>
-      </c>
-      <c r="V65" s="14">
-        <f>V63-V64</f>
-        <v>56.066000000000003</v>
-      </c>
-      <c r="W65" s="135"/>
+        <v>132</v>
+      </c>
+      <c r="H65" s="1">
+        <f>H64/H14</f>
+        <v>0.50318915060727853</v>
+      </c>
+      <c r="L65" s="1">
+        <f>L64/L14</f>
+        <v>0.77343526713555533</v>
+      </c>
+      <c r="U65" s="1">
+        <f t="shared" ref="U65:V65" si="53">U64/U14</f>
+        <v>0.63597840274765649</v>
+      </c>
+      <c r="V65" s="1">
+        <f t="shared" si="53"/>
+        <v>0.80971382354881549</v>
+      </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H67" s="1">
-        <v>1.4767999999999999</v>
-      </c>
-      <c r="L67" s="1">
-        <v>2.3904999999999998</v>
-      </c>
-      <c r="U67" s="1">
-        <v>2.395</v>
-      </c>
-      <c r="V67" s="1">
-        <v>1.8740000000000001</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H67" s="14">
+        <f t="shared" ref="H67" si="54">H44</f>
+        <v>15.635999999999999</v>
+      </c>
+      <c r="L67" s="14">
+        <f t="shared" ref="L67" si="55">L44</f>
+        <v>49.576999999999998</v>
+      </c>
+      <c r="U67" s="14">
+        <f t="shared" ref="U67" si="56">U44</f>
+        <v>29.942</v>
+      </c>
+      <c r="V67" s="14">
+        <f>V44</f>
+        <v>56.066000000000003</v>
+      </c>
+      <c r="W67" s="135"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H68" s="27">
-        <f t="shared" ref="H68" si="59">H67*H14</f>
-        <v>222.55491928799998</v>
-      </c>
-      <c r="L68" s="27">
-        <f t="shared" ref="L68" si="60">L67*L14</f>
-        <v>408.36618902800001</v>
-      </c>
-      <c r="U68" s="27">
-        <f t="shared" ref="U68" si="61">U67*U14</f>
-        <v>394.23565944500001</v>
-      </c>
-      <c r="V68" s="27">
-        <f>V67*V14</f>
-        <v>320.358961964</v>
-      </c>
-      <c r="W68" s="136"/>
+        <v>7</v>
+      </c>
+      <c r="H68" s="14">
+        <f t="shared" ref="H68" si="57">H53+H57</f>
+        <v>30.073</v>
+      </c>
+      <c r="L68" s="14">
+        <f t="shared" ref="L68" si="58">L53+L57</f>
+        <v>0</v>
+      </c>
+      <c r="U68" s="14">
+        <f t="shared" ref="U68" si="59">U53+U57</f>
+        <v>0</v>
+      </c>
+      <c r="V68" s="14">
+        <f>V53+V57</f>
+        <v>0</v>
+      </c>
+      <c r="W68" s="135"/>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H69" s="27">
-        <f>H68-H65</f>
-        <v>236.99191928799999</v>
-      </c>
-      <c r="L69" s="27">
-        <f>L68-L65</f>
-        <v>358.78918902800001</v>
-      </c>
-      <c r="U69" s="27">
-        <f>U68-U65</f>
-        <v>364.293659445</v>
-      </c>
-      <c r="V69" s="27">
-        <f>V68-V65</f>
-        <v>264.29296196400003</v>
-      </c>
-      <c r="W69" s="136"/>
-    </row>
-    <row r="71" spans="1:23" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="94" t="s">
-        <v>136</v>
-      </c>
-      <c r="E71" s="95"/>
-      <c r="G71" s="95"/>
-      <c r="H71" s="94">
-        <f>H67/H61</f>
-        <v>2.9348804484709379</v>
-      </c>
-      <c r="I71" s="95"/>
-      <c r="K71" s="95"/>
-      <c r="L71" s="94">
-        <f>L67/L61</f>
-        <v>3.0907563975629149</v>
-      </c>
-      <c r="M71" s="95"/>
-      <c r="U71" s="94">
-        <f t="shared" ref="U71" si="62">U67/U61</f>
-        <v>3.7658511510025101</v>
-      </c>
-      <c r="V71" s="94">
-        <f>V67/V61</f>
-        <v>2.3143979335645142</v>
-      </c>
-      <c r="W71" s="142"/>
-    </row>
-    <row r="72" spans="1:23" s="97" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="96"/>
-      <c r="B72" s="97" t="s">
-        <v>137</v>
-      </c>
-      <c r="E72" s="98"/>
-      <c r="G72" s="98"/>
-      <c r="I72" s="98"/>
-      <c r="K72" s="98"/>
-      <c r="M72" s="98"/>
-      <c r="U72" s="94">
-        <f t="shared" ref="U72" si="63">U68/U3</f>
-        <v>5.4847889402181478</v>
-      </c>
-      <c r="V72" s="94">
-        <f>V68/V3</f>
-        <v>1.6535424198491799</v>
-      </c>
-      <c r="W72" s="142"/>
+        <v>8</v>
+      </c>
+      <c r="H69" s="14">
+        <f>H67-H68</f>
+        <v>-14.437000000000001</v>
+      </c>
+      <c r="L69" s="14">
+        <f>L67-L68</f>
+        <v>49.576999999999998</v>
+      </c>
+      <c r="U69" s="14">
+        <f>U67-U68</f>
+        <v>29.942</v>
+      </c>
+      <c r="V69" s="14">
+        <f>V67-V68</f>
+        <v>56.066000000000003</v>
+      </c>
+      <c r="W69" s="135"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B71" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1.4767999999999999</v>
+      </c>
+      <c r="L71" s="1">
+        <v>2.3904999999999998</v>
+      </c>
+      <c r="U71" s="1">
+        <v>2.395</v>
+      </c>
+      <c r="V71" s="1">
+        <v>1.8740000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H72" s="27">
+        <f t="shared" ref="H72" si="60">H71*H14</f>
+        <v>222.55491928799998</v>
+      </c>
+      <c r="L72" s="27">
+        <f t="shared" ref="L72" si="61">L71*L14</f>
+        <v>408.36618902800001</v>
+      </c>
+      <c r="U72" s="27">
+        <f t="shared" ref="U72" si="62">U71*U14</f>
+        <v>394.23565944500001</v>
+      </c>
+      <c r="V72" s="27">
+        <f>V71*V14</f>
+        <v>320.358961964</v>
+      </c>
+      <c r="W72" s="136"/>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H73" s="27">
+        <f>H72-H69</f>
+        <v>236.99191928799999</v>
+      </c>
+      <c r="L73" s="27">
+        <f>L72-L69</f>
+        <v>358.78918902800001</v>
+      </c>
+      <c r="U73" s="27">
+        <f>U72-U69</f>
+        <v>364.293659445</v>
+      </c>
+      <c r="V73" s="27">
+        <f>V72-V69</f>
+        <v>264.29296196400003</v>
+      </c>
+      <c r="W73" s="136"/>
+    </row>
+    <row r="75" spans="1:23" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="94" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="95"/>
+      <c r="G75" s="95"/>
+      <c r="H75" s="94">
+        <f>H71/H65</f>
+        <v>2.9348804484709379</v>
+      </c>
+      <c r="I75" s="95"/>
+      <c r="K75" s="95"/>
+      <c r="L75" s="94">
+        <f>L71/L65</f>
+        <v>3.0907563975629149</v>
+      </c>
+      <c r="M75" s="95"/>
+      <c r="U75" s="94">
+        <f t="shared" ref="U75" si="63">U71/U65</f>
+        <v>3.7658511510025101</v>
+      </c>
+      <c r="V75" s="94">
+        <f>V71/V65</f>
+        <v>2.3143979335645142</v>
+      </c>
+      <c r="W75" s="142"/>
+    </row>
+    <row r="76" spans="1:23" s="97" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="96"/>
+      <c r="B76" s="97" t="s">
+        <v>135</v>
+      </c>
+      <c r="E76" s="98"/>
+      <c r="G76" s="98"/>
+      <c r="I76" s="98"/>
+      <c r="K76" s="98"/>
+      <c r="M76" s="98"/>
+      <c r="U76" s="94">
+        <f t="shared" ref="U76" si="64">U72/U3</f>
+        <v>5.4847889402181478</v>
+      </c>
+      <c r="V76" s="94">
+        <f>V72/V3</f>
+        <v>1.6535424198491799</v>
+      </c>
+      <c r="W76" s="142"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B77" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U77" s="94">
+        <f t="shared" ref="U77" si="65">U73/U3</f>
+        <v>5.0682219795347674</v>
+      </c>
+      <c r="V77" s="94">
+        <f>V73/V3</f>
+        <v>1.3641560741608643</v>
+      </c>
+      <c r="W77" s="142"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B78" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="U78" s="94">
+        <f t="shared" ref="U78" si="66">U71/U13</f>
+        <v>228.14563625289284</v>
+      </c>
+      <c r="V78" s="94">
+        <f>V71/V13</f>
+        <v>8.554082987476967</v>
+      </c>
+      <c r="W78" s="142"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B79" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="U79" s="94">
+        <f t="shared" ref="U79" si="67">U73/U12</f>
+        <v>210.81808995659659</v>
+      </c>
+      <c r="V79" s="94">
+        <f>V73/V12</f>
+        <v>7.0570335094924017</v>
+      </c>
+      <c r="W79" s="142"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B80" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="U73" s="94">
-        <f t="shared" ref="U73" si="64">U69/U3</f>
-        <v>5.0682219795347674</v>
-      </c>
-      <c r="V73" s="94">
-        <f>V69/V3</f>
-        <v>1.3641560741608643</v>
-      </c>
-      <c r="W73" s="142"/>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B74" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="U74" s="94">
-        <f t="shared" ref="U74" si="65">U67/U13</f>
-        <v>228.14563625289284</v>
-      </c>
-      <c r="V74" s="94">
-        <f>V67/V13</f>
-        <v>8.554082987476967</v>
-      </c>
-      <c r="W74" s="142"/>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B75" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="U75" s="94">
-        <f t="shared" ref="U75" si="66">U69/U12</f>
-        <v>210.81808995659659</v>
-      </c>
-      <c r="V75" s="94">
-        <f>V69/V12</f>
-        <v>7.0570335094924017</v>
-      </c>
-      <c r="W75" s="142"/>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B76" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6142,13 +6272,13 @@
         <v>44834</v>
       </c>
       <c r="B2" s="101" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q2" s="22">
         <v>44834</v>
       </c>
       <c r="R2" s="118" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -6404,10 +6534,10 @@
         <v>0.58313916923721965</v>
       </c>
       <c r="Q22" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R22" s="125" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>